<commit_message>
add details on browser compatibility to README and add widescreen test details to test cases
</commit_message>
<xml_diff>
--- a/assets/documentation/supp-spreadsheets/traceability matrix and test cases.xlsx
+++ b/assets/documentation/supp-spreadsheets/traceability matrix and test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="10515" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="10515" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -295,16 +295,17 @@
   <si>
     <t>Repeat all above tests for desktop, tablet and smartphone screens sizes.  
 a. Laptop 1920 x 1080
-b. Tablet 768 x 1024 
-c. Larger tablet 1024 x 1366
-d. Smartphone 360 x 640</t>
+b. Wide desktop 3440 x 1297
+c. Tablet 768 x 1024 
+d. Larger tablet 1024 x 1366
+e. Smartphone 360 x 640</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,21 +316,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -518,17 +504,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1050,337 +1036,338 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="72.85546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" style="15" customWidth="1"/>
-    <col min="5" max="6" width="8.28515625" style="15" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="4.85546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="10" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:6" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="E6" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="E7" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="E9" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="18" t="s">
+      <c r="E11" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="E13" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="18" t="s">
+      <c r="E14" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="18" t="s">
+      <c r="E15" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="E17" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="18" t="s">
+      <c r="E18" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="18" t="s">
+      <c r="E19" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="17" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>